<commit_message>
updated score logic and image resize function
</commit_message>
<xml_diff>
--- a/小组积分榜.xlsx
+++ b/小组积分榜.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qi.cheng\Desktop\巴伐利亚杯\网页素材\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maqiaoming/PycharmProjects/CBC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317917D7-CBC3-4E5C-A0B8-EC0F3180D415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0558596B-1285-704B-B647-14F3FD4BF31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0F306453-F322-42B6-B7DD-793AC45DF4D0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14360" activeTab="2" xr2:uid="{0F306453-F322-42B6-B7DD-793AC45DF4D0}"/>
   </bookViews>
   <sheets>
     <sheet name="A小组" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -229,623 +229,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765716</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3716</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Picture 34">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEFC55B3-1111-40E6-A9DF-EA8D03B8F85A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="611190" y="952502"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765714</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>3714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 37">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F433301-1812-42A4-A54A-0816E38C2A29}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="611188" y="1714500"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765714</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>3714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="Picture 39">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEE2125D-87C3-4C57-A7A6-234F7532E349}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="611188" y="2476500"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765714</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>3714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="Picture 41">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8554F5E-35B4-4CE3-8550-826832ED9080}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="611188" y="3238500"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765714</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7BECAB6-2CA1-40DE-8B71-4B1C09EB6C1C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="611188" y="952500"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765714</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>3714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F76C52E8-C1AB-4A95-BB24-AF613818CA1C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="611188" y="1714500"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765714</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>3714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2C27DE7-CB73-47E5-B763-9FCF23046CCA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="611188" y="2476500"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765714</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>3714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B574D30-9BA3-4CBF-924D-66640B734312}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="611188" y="3238500"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>15039</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>5013</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>773991</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1965</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{758E53A6-E8BF-4513-8EFC-66D0FBFD77DE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="626644" y="957513"/>
-          <a:ext cx="758952" cy="758952"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765714</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>3714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43962A25-AB72-4F16-8245-7D777E9B9126}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="612913" y="1714500"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765714</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>3714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D25497B4-DDBB-4BB1-81FC-ACEEE5D68D00}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="612913" y="2476500"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>765714</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>3714</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A2E647F-5D46-4D3D-A2ED-9AC421DC4BAA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="612913" y="3238500"/>
-          <a:ext cx="765714" cy="765714"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1143,19 +528,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E787F84-6832-4D9F-8431-C5D859FC1C9F}">
   <dimension ref="A2:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="11" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="11" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
         <v>13</v>
@@ -1218,7 +603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
         <v>14</v>
@@ -1251,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>15</v>
@@ -1284,7 +669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>12</v>
@@ -1323,7 +708,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1335,16 +719,16 @@
       <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="1" customWidth="1"/>
-    <col min="4" max="11" width="16.7109375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="1" customWidth="1"/>
+    <col min="4" max="11" width="16.6640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1374,7 +758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
         <v>16</v>
@@ -1407,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
         <v>10</v>
@@ -1440,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>17</v>
@@ -1473,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>18</v>
@@ -1512,7 +896,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1520,20 +903,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02FBFF1-74AF-48A2-9826-1EBD6851B20E}">
   <dimension ref="B2:K6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="1" customWidth="1"/>
-    <col min="4" max="11" width="16.7109375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="1" customWidth="1"/>
+    <col min="4" max="11" width="16.6640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1563,7 +946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
         <v>9</v>
@@ -1596,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
         <v>19</v>
@@ -1629,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>11</v>
@@ -1662,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>20</v>
@@ -1701,6 +1084,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>